<commit_message>
Update sc2 sustained production.xlsx
</commit_message>
<xml_diff>
--- a/sc2 sustained production.xlsx
+++ b/sc2 sustained production.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t xml:space="preserve">Minerals per minute:</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">Gas</t>
   </si>
   <si>
-    <t xml:space="preserve">SN</t>
+    <t xml:space="preserve">S(N)</t>
   </si>
   <si>
     <t xml:space="preserve">Seconds</t>
@@ -172,7 +172,10 @@
     <t xml:space="preserve">Queen</t>
   </si>
   <si>
-    <t xml:space="preserve">Zergling x2</t>
+    <t xml:space="preserve">Zergling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baneling</t>
   </si>
   <si>
     <t xml:space="preserve">Roach</t>
@@ -500,7 +503,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -538,6 +541,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -650,7 +657,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -2010,7 +2017,7 @@
         <v>50</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>0</v>
@@ -2023,15 +2030,15 @@
         <v>17.1428571428571</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G45" s="4" t="n">
         <f aca="false">((60/E45)*B45)/$B$1</f>
-        <v>0.194444444444444</v>
+        <v>0.0972222222222225</v>
       </c>
       <c r="H45" s="5" t="n">
         <f aca="false">((60/E45)*(B45+$F$3*F45))/$B$1</f>
-        <v>0.243055555555556</v>
+        <v>0.121527777777778</v>
       </c>
       <c r="I45" s="5" t="n">
         <f aca="false">((60/E45)*C45)/$B$2</f>
@@ -2044,32 +2051,32 @@
         <v>51</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="D46" s="0" t="n">
-        <v>27</v>
+      <c r="D46" s="10" t="n">
+        <v>44</v>
       </c>
       <c r="E46" s="3" t="n">
         <f aca="false">D46/1.4</f>
-        <v>19.2857142857143</v>
+        <v>31.4285714285714</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G46" s="4" t="n">
         <f aca="false">((60/E46)*B46)/$B$1</f>
-        <v>0.259259259259259</v>
+        <v>0.106060606060606</v>
       </c>
       <c r="H46" s="5" t="n">
         <f aca="false">((60/E46)*(B46+$F$3*F46))/$B$1</f>
-        <v>0.345679012345679</v>
+        <v>0.119318181818182</v>
       </c>
       <c r="I46" s="5" t="n">
         <f aca="false">((60/E46)*C46)/$B$2</f>
-        <v>0.243055555555555</v>
+        <v>0.149147727272727</v>
       </c>
       <c r="J46" s="6"/>
     </row>
@@ -2077,33 +2084,33 @@
       <c r="A47" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B47" s="8" t="n">
-        <v>100</v>
-      </c>
-      <c r="C47" s="8" t="n">
-        <v>100</v>
-      </c>
-      <c r="D47" s="8" t="n">
-        <v>39</v>
-      </c>
-      <c r="E47" s="9" t="n">
+      <c r="B47" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="E47" s="3" t="n">
         <f aca="false">D47/1.4</f>
-        <v>27.8571428571429</v>
-      </c>
-      <c r="F47" s="8" t="n">
-        <v>3</v>
+        <v>19.2857142857143</v>
+      </c>
+      <c r="F47" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="G47" s="4" t="n">
         <f aca="false">((60/E47)*B47)/$B$1</f>
-        <v>0.239316239316239</v>
+        <v>0.259259259259259</v>
       </c>
       <c r="H47" s="5" t="n">
         <f aca="false">((60/E47)*(B47+$F$3*F47))/$B$1</f>
-        <v>0.329059829059829</v>
+        <v>0.345679012345679</v>
       </c>
       <c r="I47" s="5" t="n">
         <f aca="false">((60/E47)*C47)/$B$2</f>
-        <v>0.673076923076923</v>
+        <v>0.243055555555555</v>
       </c>
       <c r="J47" s="6"/>
     </row>
@@ -2111,33 +2118,33 @@
       <c r="A48" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="8" t="n">
         <v>100</v>
       </c>
-      <c r="C48" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="D48" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="E48" s="3" t="n">
+      <c r="C48" s="8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D48" s="8" t="n">
+        <v>39</v>
+      </c>
+      <c r="E48" s="9" t="n">
         <f aca="false">D48/1.4</f>
-        <v>23.5714285714286</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>2</v>
+        <v>27.8571428571429</v>
+      </c>
+      <c r="F48" s="8" t="n">
+        <v>3</v>
       </c>
       <c r="G48" s="4" t="n">
         <f aca="false">((60/E48)*B48)/$B$1</f>
-        <v>0.282828282828283</v>
+        <v>0.239316239316239</v>
       </c>
       <c r="H48" s="5" t="n">
         <f aca="false">((60/E48)*(B48+$F$3*F48))/$B$1</f>
-        <v>0.353535353535353</v>
+        <v>0.329059829059829</v>
       </c>
       <c r="I48" s="5" t="n">
         <f aca="false">((60/E48)*C48)/$B$2</f>
-        <v>0.397727272727273</v>
+        <v>0.673076923076923</v>
       </c>
       <c r="J48" s="6"/>
     </row>
@@ -2145,33 +2152,33 @@
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="8" t="n">
-        <v>150</v>
-      </c>
-      <c r="C49" s="8" t="n">
-        <v>150</v>
-      </c>
-      <c r="D49" s="8" t="n">
-        <v>58</v>
-      </c>
-      <c r="E49" s="9" t="n">
+      <c r="B49" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="E49" s="3" t="n">
         <f aca="false">D49/1.4</f>
-        <v>41.4285714285714</v>
-      </c>
-      <c r="F49" s="8" t="n">
-        <v>3</v>
+        <v>23.5714285714286</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="G49" s="4" t="n">
         <f aca="false">((60/E49)*B49)/$B$1</f>
-        <v>0.241379310344828</v>
+        <v>0.282828282828283</v>
       </c>
       <c r="H49" s="5" t="n">
         <f aca="false">((60/E49)*(B49+$F$3*F49))/$B$1</f>
-        <v>0.301724137931034</v>
+        <v>0.353535353535353</v>
       </c>
       <c r="I49" s="5" t="n">
         <f aca="false">((60/E49)*C49)/$B$2</f>
-        <v>0.678879310344828</v>
+        <v>0.397727272727273</v>
       </c>
       <c r="J49" s="6"/>
     </row>
@@ -2179,33 +2186,33 @@
       <c r="A50" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="C50" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="D50" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="E50" s="3" t="n">
+      <c r="B50" s="8" t="n">
+        <v>150</v>
+      </c>
+      <c r="C50" s="8" t="n">
+        <v>150</v>
+      </c>
+      <c r="D50" s="8" t="n">
+        <v>58</v>
+      </c>
+      <c r="E50" s="9" t="n">
         <f aca="false">D50/1.4</f>
-        <v>23.5714285714286</v>
-      </c>
-      <c r="F50" s="0" t="n">
-        <v>2</v>
+        <v>41.4285714285714</v>
+      </c>
+      <c r="F50" s="8" t="n">
+        <v>3</v>
       </c>
       <c r="G50" s="4" t="n">
         <f aca="false">((60/E50)*B50)/$B$1</f>
-        <v>0.282828282828283</v>
+        <v>0.241379310344828</v>
       </c>
       <c r="H50" s="5" t="n">
         <f aca="false">((60/E50)*(B50+$F$3*F50))/$B$1</f>
-        <v>0.353535353535353</v>
+        <v>0.301724137931034</v>
       </c>
       <c r="I50" s="5" t="n">
         <f aca="false">((60/E50)*C50)/$B$2</f>
-        <v>0.795454545454545</v>
+        <v>0.678879310344828</v>
       </c>
       <c r="J50" s="6"/>
     </row>
@@ -2214,32 +2221,32 @@
         <v>56</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>100</v>
       </c>
       <c r="D51" s="0" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E51" s="3" t="n">
         <f aca="false">D51/1.4</f>
-        <v>28.5714285714286</v>
+        <v>23.5714285714286</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G51" s="4" t="n">
         <f aca="false">((60/E51)*B51)/$B$1</f>
-        <v>0.35</v>
+        <v>0.282828282828283</v>
       </c>
       <c r="H51" s="5" t="n">
         <f aca="false">((60/E51)*(B51+$F$3*F51))/$B$1</f>
-        <v>0.408333333333333</v>
+        <v>0.353535353535353</v>
       </c>
       <c r="I51" s="5" t="n">
         <f aca="false">((60/E51)*C51)/$B$2</f>
-        <v>0.65625</v>
+        <v>0.795454545454545</v>
       </c>
       <c r="J51" s="6"/>
     </row>
@@ -2247,33 +2254,33 @@
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="8" t="n">
-        <v>300</v>
-      </c>
-      <c r="C52" s="8" t="n">
-        <v>250</v>
-      </c>
-      <c r="D52" s="8" t="n">
-        <v>74</v>
-      </c>
-      <c r="E52" s="9" t="n">
+      <c r="B52" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="E52" s="3" t="n">
         <f aca="false">D52/1.4</f>
-        <v>52.8571428571429</v>
-      </c>
-      <c r="F52" s="8" t="n">
-        <v>4</v>
+        <v>28.5714285714286</v>
+      </c>
+      <c r="F52" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="G52" s="4" t="n">
         <f aca="false">((60/E52)*B52)/$B$1</f>
-        <v>0.378378378378378</v>
+        <v>0.35</v>
       </c>
       <c r="H52" s="5" t="n">
         <f aca="false">((60/E52)*(B52+$F$3*F52))/$B$1</f>
-        <v>0.441441441441441</v>
+        <v>0.408333333333333</v>
       </c>
       <c r="I52" s="5" t="n">
         <f aca="false">((60/E52)*C52)/$B$2</f>
-        <v>0.886824324324324</v>
+        <v>0.65625</v>
       </c>
       <c r="J52" s="6"/>
     </row>
@@ -2281,33 +2288,33 @@
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="C53" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="D53" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="E53" s="3" t="n">
+      <c r="B53" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="C53" s="8" t="n">
+        <v>250</v>
+      </c>
+      <c r="D53" s="8" t="n">
+        <v>74</v>
+      </c>
+      <c r="E53" s="9" t="n">
         <f aca="false">D53/1.4</f>
-        <v>35.7142857142857</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <v>2</v>
+        <v>52.8571428571429</v>
+      </c>
+      <c r="F53" s="8" t="n">
+        <v>4</v>
       </c>
       <c r="G53" s="4" t="n">
         <f aca="false">((60/E53)*B53)/$B$1</f>
-        <v>0.186666666666667</v>
+        <v>0.378378378378378</v>
       </c>
       <c r="H53" s="5" t="n">
         <f aca="false">((60/E53)*(B53+$F$3*F53))/$B$1</f>
-        <v>0.233333333333333</v>
+        <v>0.441441441441441</v>
       </c>
       <c r="I53" s="5" t="n">
         <f aca="false">((60/E53)*C53)/$B$2</f>
-        <v>0.7875</v>
+        <v>0.886824324324324</v>
       </c>
       <c r="J53" s="6"/>
     </row>
@@ -2319,29 +2326,29 @@
         <v>100</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E54" s="3" t="n">
         <f aca="false">D54/1.4</f>
-        <v>28.5714285714286</v>
+        <v>35.7142857142857</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G54" s="4" t="n">
         <f aca="false">((60/E54)*B54)/$B$1</f>
-        <v>0.233333333333333</v>
+        <v>0.186666666666667</v>
       </c>
       <c r="H54" s="5" t="n">
         <f aca="false">((60/E54)*(B54+$F$3*F54))/$B$1</f>
-        <v>0.320833333333333</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="I54" s="5" t="n">
         <f aca="false">((60/E54)*C54)/$B$2</f>
-        <v>0.4921875</v>
+        <v>0.7875</v>
       </c>
       <c r="J54" s="6"/>
     </row>
@@ -2353,7 +2360,7 @@
         <v>100</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>200</v>
+        <v>75</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>40</v>
@@ -2375,7 +2382,7 @@
       </c>
       <c r="I55" s="5" t="n">
         <f aca="false">((60/E55)*C55)/$B$2</f>
-        <v>1.3125</v>
+        <v>0.4921875</v>
       </c>
       <c r="J55" s="6"/>
     </row>
@@ -2384,41 +2391,74 @@
         <v>61</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>200</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E56" s="3" t="n">
         <f aca="false">D56/1.4</f>
-        <v>39.2857142857143</v>
+        <v>28.5714285714286</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G56" s="4" t="n">
         <f aca="false">((60/E56)*B56)/$B$1</f>
-        <v>0.509090909090909</v>
+        <v>0.233333333333333</v>
       </c>
       <c r="H56" s="5" t="n">
         <f aca="false">((60/E56)*(B56+$F$3*F56))/$B$1</f>
-        <v>0.636363636363636</v>
+        <v>0.320833333333333</v>
       </c>
       <c r="I56" s="5" t="n">
         <f aca="false">((60/E56)*C56)/$B$2</f>
+        <v>1.3125</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <f aca="false">D57/1.4</f>
+        <v>39.2857142857143</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G57" s="4" t="n">
+        <f aca="false">((60/E57)*B57)/$B$1</f>
+        <v>0.509090909090909</v>
+      </c>
+      <c r="H57" s="5" t="n">
+        <f aca="false">((60/E57)*(B57+$F$3*F57))/$B$1</f>
+        <v>0.636363636363636</v>
+      </c>
+      <c r="I57" s="5" t="n">
+        <f aca="false">((60/E57)*C57)/$B$2</f>
         <v>0.954545454545455</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H6:H56">
+  <conditionalFormatting sqref="H6:H57">
     <cfRule type="cellIs" priority="2" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6:I56">
+  <conditionalFormatting sqref="I6:I57">
     <cfRule type="cellIs" priority="3" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H6</formula>
     </cfRule>

</xml_diff>